<commit_message>
add edit and delete feature
</commit_message>
<xml_diff>
--- a/public/datas/Items.xlsx
+++ b/public/datas/Items.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Sl.no.</t>
   </si>
@@ -74,6 +74,33 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>Www</t>
+  </si>
+  <si>
+    <t>Sss</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>Ass</t>
+  </si>
+  <si>
+    <t>44565655</t>
+  </si>
+  <si>
+    <t>ggrgr</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>WITH GROOVE plus with gropve</t>
+  </si>
+  <si>
+    <t>acrylic</t>
   </si>
 </sst>
 </file>
@@ -460,10 +487,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+  <dimension ref="A1:K13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
@@ -721,6 +745,216 @@
         <v>2253</v>
       </c>
     </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>664</v>
+      </c>
+      <c r="E8">
+        <v>540</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>7.719</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8">
+        <v>280</v>
+      </c>
+      <c r="K8">
+        <v>2161.32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>550</v>
+      </c>
+      <c r="E9">
+        <v>700</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <v>12.432</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9">
+        <v>256</v>
+      </c>
+      <c r="K9">
+        <v>3182.592</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>550</v>
+      </c>
+      <c r="E10">
+        <v>700</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>12.432</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10">
+        <v>256</v>
+      </c>
+      <c r="K10">
+        <v>3182.592</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>550</v>
+      </c>
+      <c r="E11">
+        <v>600</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>10.656</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11">
+        <v>300</v>
+      </c>
+      <c r="K11">
+        <v>3196.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>123456</v>
+      </c>
+      <c r="D12">
+        <v>123456</v>
+      </c>
+      <c r="E12">
+        <v>123456</v>
+      </c>
+      <c r="F12">
+        <v>123456</v>
+      </c>
+      <c r="G12">
+        <v>20253807542.593</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12">
+        <v>123456</v>
+      </c>
+      <c r="K12">
+        <v>2500454063978361</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>444</v>
+      </c>
+      <c r="D13">
+        <v>444</v>
+      </c>
+      <c r="E13">
+        <v>4435345</v>
+      </c>
+      <c r="F13">
+        <v>435343</v>
+      </c>
+      <c r="G13">
+        <v>9228094145.572</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13">
+        <v>3333</v>
+      </c>
+      <c r="K13">
+        <v>30757237787191.477</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
made job card system
partially done, done other necessary changes
</commit_message>
<xml_diff>
--- a/public/datas/Items.xlsx
+++ b/public/datas/Items.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Sl.no.</t>
   </si>
@@ -46,61 +46,37 @@
     <t>Amount</t>
   </si>
   <si>
+    <t>new carcase</t>
+  </si>
+  <si>
+    <t>WITH GROVE</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
     <t>carcase</t>
   </si>
   <si>
-    <t>SHELF</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>new carcase</t>
-  </si>
-  <si>
-    <t>WITH GROVE</t>
+    <t>WITH GROOVe</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
   <si>
     <t>WITH GROOVE</t>
   </si>
   <si>
-    <t>11</t>
+    <t>0</t>
   </si>
   <si>
     <t>car case</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Www</t>
-  </si>
-  <si>
-    <t>Sss</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>Ass</t>
-  </si>
-  <si>
-    <t>44565655</t>
-  </si>
-  <si>
-    <t>ggrgr</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>WITH GROOVE plus with gropve</t>
-  </si>
-  <si>
-    <t>acrylic</t>
+    <t>grove</t>
+  </si>
+  <si>
+    <t>itali</t>
   </si>
 </sst>
 </file>
@@ -487,7 +463,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
@@ -546,16 +522,16 @@
         <v>18</v>
       </c>
       <c r="D2">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="E2">
-        <v>234</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
       <c r="G2">
-        <v>0.605</v>
+        <v>0.005</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -564,10 +540,10 @@
         <v>13</v>
       </c>
       <c r="J2">
-        <v>290</v>
+        <v>250</v>
       </c>
       <c r="K2">
-        <v>175.45</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -578,31 +554,31 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3">
-        <v>20</v>
+        <v>1230</v>
       </c>
       <c r="E3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>222</v>
       </c>
       <c r="G3">
-        <v>0.005</v>
+        <v>5.878</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J3">
-        <v>250</v>
+        <v>10</v>
       </c>
       <c r="K3">
-        <v>1.25</v>
+        <v>58.78</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -616,28 +592,28 @@
         <v>18</v>
       </c>
       <c r="D4">
-        <v>120</v>
+        <v>456</v>
       </c>
       <c r="E4">
-        <v>230</v>
+        <v>765</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4">
-        <v>0.594</v>
+        <v>7.51</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J4">
-        <v>123</v>
+        <v>300</v>
       </c>
       <c r="K4">
-        <v>73.062</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -645,34 +621,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
         <v>18</v>
       </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
       <c r="D5">
-        <v>22</v>
+        <v>664</v>
       </c>
       <c r="E5">
-        <v>22</v>
+        <v>540</v>
       </c>
       <c r="F5">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>0.115</v>
+        <v>7.719</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="J5">
-        <v>222</v>
+        <v>280</v>
       </c>
       <c r="K5">
-        <v>25.53</v>
+        <v>2161.32</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -680,279 +656,34 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D6">
+        <v>540</v>
+      </c>
+      <c r="E6">
+        <v>664</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>11.579</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6">
         <v>123</v>
       </c>
-      <c r="E6">
-        <v>432</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>1.144</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6">
-        <v>111</v>
-      </c>
       <c r="K6">
-        <v>126.984</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>18</v>
-      </c>
-      <c r="D7">
-        <v>456</v>
-      </c>
-      <c r="E7">
-        <v>765</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>7.51</v>
-      </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7">
-        <v>300</v>
-      </c>
-      <c r="K7">
-        <v>2253</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>664</v>
-      </c>
-      <c r="E8">
-        <v>540</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>7.719</v>
-      </c>
-      <c r="H8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8">
-        <v>280</v>
-      </c>
-      <c r="K8">
-        <v>2161.32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9">
-        <v>12</v>
-      </c>
-      <c r="D9">
-        <v>550</v>
-      </c>
-      <c r="E9">
-        <v>700</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <v>12.432</v>
-      </c>
-      <c r="H9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9">
-        <v>256</v>
-      </c>
-      <c r="K9">
-        <v>3182.592</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10">
-        <v>12</v>
-      </c>
-      <c r="D10">
-        <v>550</v>
-      </c>
-      <c r="E10">
-        <v>700</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10">
-        <v>12.432</v>
-      </c>
-      <c r="H10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10">
-        <v>256</v>
-      </c>
-      <c r="K10">
-        <v>3182.592</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11">
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>550</v>
-      </c>
-      <c r="E11">
-        <v>600</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <v>10.656</v>
-      </c>
-      <c r="H11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11">
-        <v>300</v>
-      </c>
-      <c r="K11">
-        <v>3196.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12">
-        <v>123456</v>
-      </c>
-      <c r="D12">
-        <v>123456</v>
-      </c>
-      <c r="E12">
-        <v>123456</v>
-      </c>
-      <c r="F12">
-        <v>123456</v>
-      </c>
-      <c r="G12">
-        <v>20253807542.593</v>
-      </c>
-      <c r="H12" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J12">
-        <v>123456</v>
-      </c>
-      <c r="K12">
-        <v>2500454063978361</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13">
-        <v>444</v>
-      </c>
-      <c r="D13">
-        <v>444</v>
-      </c>
-      <c r="E13">
-        <v>4435345</v>
-      </c>
-      <c r="F13">
-        <v>435343</v>
-      </c>
-      <c r="G13">
-        <v>9228094145.572</v>
-      </c>
-      <c r="H13" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" t="s">
-        <v>29</v>
-      </c>
-      <c r="J13">
-        <v>3333</v>
-      </c>
-      <c r="K13">
-        <v>30757237787191.477</v>
+        <v>1424.217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix auto-calculate issue, add item issue
</commit_message>
<xml_diff>
--- a/public/datas/Items.xlsx
+++ b/public/datas/Items.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Sl.no.</t>
   </si>
@@ -44,39 +44,6 @@
   </si>
   <si>
     <t>Amount</t>
-  </si>
-  <si>
-    <t>new carcase</t>
-  </si>
-  <si>
-    <t>WITH GROVE</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>carcase</t>
-  </si>
-  <si>
-    <t>WITH GROOVe</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>WITH GROOVE</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>car case</t>
-  </si>
-  <si>
-    <t>grove</t>
-  </si>
-  <si>
-    <t>itali</t>
   </si>
 </sst>
 </file>
@@ -463,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
@@ -511,179 +478,34 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>18</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2">
-        <v>12</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>0.005</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2">
-        <v>250</v>
-      </c>
-      <c r="K2">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3">
-        <v>19</v>
-      </c>
-      <c r="D3">
-        <v>1230</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>222</v>
-      </c>
-      <c r="G3">
-        <v>5.878</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3">
-        <v>10</v>
-      </c>
-      <c r="K3">
-        <v>58.78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4">
-        <v>18</v>
-      </c>
-      <c r="D4">
-        <v>456</v>
-      </c>
-      <c r="E4">
-        <v>765</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>7.51</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4">
-        <v>300</v>
-      </c>
-      <c r="K4">
-        <v>2253</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>18</v>
-      </c>
-      <c r="D5">
-        <v>664</v>
-      </c>
-      <c r="E5">
-        <v>540</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>7.719</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5">
-        <v>280</v>
-      </c>
-      <c r="K5">
-        <v>2161.32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>18</v>
-      </c>
-      <c r="D6">
-        <v>540</v>
-      </c>
-      <c r="E6">
-        <v>664</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>11.579</v>
-      </c>
-      <c r="H6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6">
-        <v>123</v>
-      </c>
-      <c r="K6">
-        <v>1424.217</v>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix delete an Item in job card
</commit_message>
<xml_diff>
--- a/public/datas/Items.xlsx
+++ b/public/datas/Items.xlsx
@@ -430,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
@@ -483,29 +483,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
+      <c r="G3">
+        <v>7.719</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
+      </c>
+      <c r="G4">
+        <v>11.579</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>